<commit_message>
get translation"s root info with root pecha id
</commit_message>
<xml_diff>
--- a/tests/pecha/parser/google_doc/translation/data/bo/Tibetan Root text Translation Metadata.xlsx
+++ b/tests/pecha/parser/google_doc/translation/data/bo/Tibetan Root text Translation Metadata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\tsundue\mywork\toolkit-v2\tests\pecha\parser\google_doc\translation\data\bo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\tsundue\mycodes\toolkit-v2\tests\pecha\parser\google_doc\translation\data\bo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8651EFEE-8351-444B-9492-2D1B929E52B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97AB0E6A-F7A4-45E1-BE77-8D579ED7B5D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -85,16 +85,16 @@
     <t>title_alt_5</t>
   </si>
   <si>
-    <t>is_commentary_of</t>
-  </si>
-  <si>
-    <t>is_version_of</t>
-  </si>
-  <si>
     <t>language</t>
   </si>
   <si>
     <t>bo</t>
+  </si>
+  <si>
+    <t>translation_of</t>
+  </si>
+  <si>
+    <t>commentary_of</t>
   </si>
 </sst>
 </file>
@@ -570,12 +570,12 @@
   <dimension ref="A1:W1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:23" ht="12.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -635,7 +635,7 @@
       <c r="V2" s="2"/>
       <c r="W2" s="2"/>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:23" ht="15">
       <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
@@ -662,7 +662,7 @@
       <c r="V3" s="2"/>
       <c r="W3" s="2"/>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:23" ht="15">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -689,7 +689,7 @@
       <c r="V4" s="2"/>
       <c r="W4" s="2"/>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:23" ht="15">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -716,7 +716,7 @@
       <c r="V5" s="2"/>
       <c r="W5" s="2"/>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:23" ht="15">
       <c r="A6" s="9" t="s">
         <v>8</v>
       </c>
@@ -743,7 +743,7 @@
       <c r="V6" s="2"/>
       <c r="W6" s="2"/>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:23" ht="16.5">
       <c r="A7" s="11" t="s">
         <v>9</v>
       </c>
@@ -774,7 +774,7 @@
       <c r="V7" s="2"/>
       <c r="W7" s="2"/>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:23" ht="49.5">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
@@ -803,7 +803,7 @@
       <c r="V8" s="2"/>
       <c r="W8" s="2"/>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:23" ht="15">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -832,7 +832,7 @@
       <c r="V9" s="2"/>
       <c r="W9" s="2"/>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:23" ht="15">
       <c r="A10" s="9" t="s">
         <v>16</v>
       </c>
@@ -861,7 +861,7 @@
       <c r="V10" s="2"/>
       <c r="W10" s="2"/>
     </row>
-    <row r="11" spans="1:23">
+    <row r="11" spans="1:23" ht="15">
       <c r="A11" s="6" t="s">
         <v>18</v>
       </c>
@@ -888,7 +888,7 @@
       <c r="V11" s="2"/>
       <c r="W11" s="2"/>
     </row>
-    <row r="12" spans="1:23">
+    <row r="12" spans="1:23" ht="15">
       <c r="A12" s="9" t="s">
         <v>19</v>
       </c>
@@ -915,7 +915,7 @@
       <c r="V12" s="2"/>
       <c r="W12" s="2"/>
     </row>
-    <row r="13" spans="1:23">
+    <row r="13" spans="1:23" ht="15">
       <c r="A13" s="6" t="s">
         <v>20</v>
       </c>
@@ -942,9 +942,9 @@
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
     </row>
-    <row r="14" spans="1:23">
+    <row r="14" spans="1:23" ht="15">
       <c r="A14" s="15" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B14" s="16"/>
       <c r="C14" s="2"/>
@@ -969,9 +969,9 @@
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
     </row>
-    <row r="15" spans="1:23">
+    <row r="15" spans="1:23" ht="15">
       <c r="A15" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B15" s="18"/>
       <c r="C15" s="2"/>
@@ -996,12 +996,12 @@
       <c r="V15" s="2"/>
       <c r="W15" s="2"/>
     </row>
-    <row r="16" spans="1:23">
+    <row r="16" spans="1:23" ht="15">
       <c r="A16" s="19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -1025,7 +1025,7 @@
       <c r="V16" s="2"/>
       <c r="W16" s="2"/>
     </row>
-    <row r="17" spans="1:23">
+    <row r="17" spans="1:23" ht="12.75">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1050,7 +1050,7 @@
       <c r="V17" s="2"/>
       <c r="W17" s="2"/>
     </row>
-    <row r="18" spans="1:23">
+    <row r="18" spans="1:23" ht="12.75">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1075,7 +1075,7 @@
       <c r="V18" s="2"/>
       <c r="W18" s="2"/>
     </row>
-    <row r="19" spans="1:23">
+    <row r="19" spans="1:23" ht="12.75">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>

</xml_diff>